<commit_message>
Updated timelines and alternative formats
</commit_message>
<xml_diff>
--- a/images/alternative/Technology-context.xlsx
+++ b/images/alternative/Technology-context.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\MASH-EHC\sigma\keynote\Timeline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA957FD2-8A08-448C-B767-F096AE0C8A18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E7E4776-8A4E-4704-A1DC-DBCC11D48281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Technology context" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Technology context'!$A$1:$E$12</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="43">
   <si>
     <t>Date</t>
   </si>
@@ -139,6 +139,24 @@
   </si>
   <si>
     <t>Student capability enhanced</t>
+  </si>
+  <si>
+    <t>Desmos accessibility</t>
+  </si>
+  <si>
+    <t>https://blog.desmos.com/articles/friday-fave-for-november-2/</t>
+  </si>
+  <si>
+    <t>https://wiki.geogebra.org/en/Accessibility</t>
+  </si>
+  <si>
+    <t>Geogebra 5.0</t>
+  </si>
+  <si>
+    <t>BrailleR</t>
+  </si>
+  <si>
+    <t>https://cran.r-project.org/web/packages/BrailleR/index.html</t>
   </si>
 </sst>
 </file>
@@ -495,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -725,37 +743,80 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
-        <v>42536</v>
-      </c>
-      <c r="B15" s="4"/>
+        <v>41885</v>
+      </c>
       <c r="C15" s="5" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>36</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
-        <v>42793</v>
-      </c>
-      <c r="B16" s="4"/>
+        <v>42094</v>
+      </c>
       <c r="C16" s="5" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>36</v>
       </c>
       <c r="E16" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="4">
+        <v>42536</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="4">
+        <v>42793</v>
+      </c>
+      <c r="B18" s="4"/>
+      <c r="C18" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="4">
+        <v>43345</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:E12" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E16">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E19">
       <sortCondition ref="A1:A12"/>
     </sortState>
   </autoFilter>
@@ -768,12 +829,15 @@
     <hyperlink ref="E12" r:id="rId6" location="Version_3.0.1" xr:uid="{3C831621-FAB7-4B8A-A666-7DD4A3CF024C}"/>
     <hyperlink ref="E13" r:id="rId7" xr:uid="{84E94488-B769-4588-84B1-8464093BB4A8}"/>
     <hyperlink ref="E14" r:id="rId8" xr:uid="{B6E1212C-0D7C-479E-A30F-D6C4C6F08495}"/>
-    <hyperlink ref="E15" r:id="rId9" xr:uid="{FE058256-884C-4545-95C0-81C0C7836C34}"/>
-    <hyperlink ref="E16" r:id="rId10" xr:uid="{A3EEF17F-DEAD-4C77-9A3F-C2563E962419}"/>
+    <hyperlink ref="E17" r:id="rId9" xr:uid="{FE058256-884C-4545-95C0-81C0C7836C34}"/>
+    <hyperlink ref="E18" r:id="rId10" xr:uid="{A3EEF17F-DEAD-4C77-9A3F-C2563E962419}"/>
     <hyperlink ref="E3" r:id="rId11" xr:uid="{FB2B5C05-4798-4A2E-A9E6-3C0CE5C682F6}"/>
     <hyperlink ref="E10" r:id="rId12" xr:uid="{E4D19697-5CA2-4733-B84E-FCE6C5AC07CC}"/>
     <hyperlink ref="E7" r:id="rId13" xr:uid="{2409AB7D-A202-4619-8834-0B4C68E44B1A}"/>
     <hyperlink ref="E2" r:id="rId14" xr:uid="{9106CA65-1A67-40F1-BA1D-81C1C8983CE3}"/>
+    <hyperlink ref="E19" r:id="rId15" xr:uid="{BFCF8E25-E5D9-4D9B-83F1-4EDAF79124AD}"/>
+    <hyperlink ref="E15" r:id="rId16" xr:uid="{4E4761DC-A633-47B1-A570-18553FB1873F}"/>
+    <hyperlink ref="E16" r:id="rId17" xr:uid="{70CDC4F9-9226-456E-AACF-80482A6370B9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>